<commit_message>
update to batpac v5
</commit_message>
<xml_diff>
--- a/batt_sust_model/data/battery_design_parameters.xlsx
+++ b/batt_sust_model/data/battery_design_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b8061896_newcastle_ac_uk/Documents/Python/Projects/IM_SMS_Batt/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b8061896_newcastle_ac_uk/Documents/Python/Projects/Batt_Sust_Model/batt_sust_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="433" documentId="13_ncr:1_{1150D49F-0BD8-4425-B7C3-9A96F042F7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{755584EC-75B5-4888-80D3-307094396BE1}"/>
+  <xr:revisionPtr revIDLastSave="440" documentId="13_ncr:1_{1150D49F-0BD8-4425-B7C3-9A96F042F7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E982DCFF-170F-47AE-8B45-359673DEF2F9}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{0E16CDF7-5CB0-4173-9C6D-D5B194B1AB4C}"/>
   </bookViews>
@@ -19,9 +19,8 @@
     <sheet name="pack_parameters" sheetId="6" r:id="rId4"/>
     <sheet name="module_parameters" sheetId="4" r:id="rId5"/>
     <sheet name="cell_parameters" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="266">
   <si>
     <t>Unit</t>
   </si>
@@ -327,9 +326,6 @@
     <t>minutes</t>
   </si>
   <si>
-    <t>calculated_fast_charge</t>
-  </si>
-  <si>
     <t>max_charge_density</t>
   </si>
   <si>
@@ -366,18 +362,9 @@
     <t>The thickness of the separator ceramic coating</t>
   </si>
   <si>
-    <t>5,7,9</t>
-  </si>
-  <si>
     <t>sep_coat_thickness</t>
   </si>
   <si>
-    <t>sep_foil_thickness</t>
-  </si>
-  <si>
-    <t>0,2,3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Percentage of CMC in the anode binder </t>
   </si>
   <si>
@@ -442,22 +429,6 @@
   </si>
   <si>
     <t>drivetrain</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If yes, includes fast charging, resulting in lower loading design to prevent Li platting. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Only for EV vehicle types</t>
-    </r>
   </si>
   <si>
     <t>Contains all battery design parameter names and value ranges that can be changed.</t>
@@ -710,54 +681,6 @@
   </si>
   <si>
     <t>integer,float</t>
-  </si>
-  <si>
-    <t>NMC333-G (Power),NMC532-G,NMC622-G,NMC811-G,NCA-G,LFP-G,LMO-G,NMC532/50%/LMO  - G</t>
-  </si>
-  <si>
-    <t>NMC333-G (Power)</t>
-  </si>
-  <si>
-    <t>NMC333-G (Energy)</t>
-  </si>
-  <si>
-    <t>NMC532-G (Power)</t>
-  </si>
-  <si>
-    <t>NMC532-G (Energy)</t>
-  </si>
-  <si>
-    <t>NMC622-G (Power)</t>
-  </si>
-  <si>
-    <t>NMC622-G (Energy)</t>
-  </si>
-  <si>
-    <t>NMC811-G (Power)</t>
-  </si>
-  <si>
-    <t>NMC811-G (Energy)</t>
-  </si>
-  <si>
-    <t>NCA-G (Power)</t>
-  </si>
-  <si>
-    <t>NCA-G (Energy)</t>
-  </si>
-  <si>
-    <t>LFP-G (Power)</t>
-  </si>
-  <si>
-    <t>LFP-G (Energy)</t>
-  </si>
-  <si>
-    <t>LMO-G (Power)</t>
-  </si>
-  <si>
-    <t>LMO-G (Energy)</t>
-  </si>
-  <si>
-    <t>50%/50% NMC532/LMO - G</t>
   </si>
   <si>
     <t>NMC333-G (Power),NMC333-G (Energy),NMC532-G (Power),NMC532-G (Energy),NMC622-G (Power),NMC622-G (Energy),NMC811-G (Power),NMC811-G (Energy),NCA-G (Power),NCA-G (Energy),LFP-G (Power),LFP-G (Energy),LMO-G (Power),LMO-G (Energy),50%/50% NMC532/LMO - G</t>
@@ -974,6 +897,34 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>sep_film_thickness</t>
+  </si>
+  <si>
+    <t>5,6,7,8,9,10,11,12,13,14,15</t>
+  </si>
+  <si>
+    <t>0,1,2,3</t>
+  </si>
+  <si>
+    <t>calculate_fast_charge</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If yes, includes fast charging, resulting in lower loading design to prevent Li platting. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Only for BEV and PHEV vehicle types</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1447,12 +1398,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25">
       <c r="A1" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="23.25">
       <c r="A2" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1477,10 +1428,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -1509,10 +1460,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -1535,13 +1486,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1572,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD76366C-A7A1-48C8-88C5-2E677A1AC493}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1592,10 +1543,10 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -1616,7 +1567,7 @@
         <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -1627,7 +1578,7 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -1656,7 +1607,7 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
         <v>71</v>
@@ -1665,7 +1616,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -1685,7 +1636,7 @@
         <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>88</v>
@@ -1697,10 +1648,10 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="G4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="H4">
         <v>37</v>
@@ -1714,10 +1665,10 @@
         <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -1743,7 +1694,7 @@
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>93</v>
@@ -1769,19 +1720,19 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>95</v>
+        <v>264</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>265</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -1795,13 +1746,13 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -1819,18 +1770,18 @@
         <v>240</v>
       </c>
       <c r="J8" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -1848,15 +1799,15 @@
         <v>239</v>
       </c>
       <c r="J9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -1877,7 +1828,7 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1885,7 +1836,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>73</v>
@@ -1894,7 +1845,7 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -1907,107 +1858,107 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H12" s="3">
         <v>2</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H13" s="3">
         <v>3</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18.75" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H14">
         <v>4</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>29</v>
@@ -2016,39 +1967,39 @@
         <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H15">
         <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H16">
         <v>14</v>
@@ -2062,25 +2013,25 @@
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1">
       <c r="A17" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H17" s="3">
         <v>15</v>
@@ -2094,25 +2045,25 @@
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1">
       <c r="A18" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H18" s="3">
         <v>16</v>
@@ -2126,25 +2077,25 @@
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1">
       <c r="A19" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H19" s="3">
         <v>30</v>
@@ -2158,25 +2109,25 @@
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1">
       <c r="A20" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H20" s="3">
         <v>31</v>
@@ -2190,25 +2141,25 @@
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1">
       <c r="A21" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H21" s="3">
         <v>32</v>
@@ -2222,25 +2173,25 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1">
       <c r="A22" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H22" s="3">
         <v>33</v>
@@ -2254,25 +2205,25 @@
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1">
       <c r="A23" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H23" s="3">
         <v>34</v>
@@ -2286,25 +2237,25 @@
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1">
       <c r="A24" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H24" s="3">
         <v>25</v>
@@ -2318,13 +2269,13 @@
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1">
       <c r="A25" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>29</v>
@@ -2333,10 +2284,10 @@
         <v>26</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H25" s="3">
         <v>36</v>
@@ -2345,30 +2296,30 @@
         <v>750</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1">
       <c r="A26" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H26" s="3">
         <v>38</v>
@@ -2382,25 +2333,25 @@
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H27" s="3">
         <v>39</v>
@@ -2414,13 +2365,13 @@
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>29</v>
@@ -2429,10 +2380,10 @@
         <v>26</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H28" s="3">
         <v>44</v>
@@ -2441,18 +2392,18 @@
         <v>2098</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>29</v>
@@ -2461,10 +2412,10 @@
         <v>26</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H29" s="3">
         <v>44</v>
@@ -2473,18 +2424,18 @@
         <v>1165</v>
       </c>
       <c r="J29" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>29</v>
@@ -2493,10 +2444,10 @@
         <v>26</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H30" s="3">
         <v>45</v>
@@ -2505,18 +2456,18 @@
         <v>11990</v>
       </c>
       <c r="J30" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>29</v>
@@ -2525,10 +2476,10 @@
         <v>26</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H31" s="3">
         <v>45</v>
@@ -2537,18 +2488,18 @@
         <v>16507</v>
       </c>
       <c r="J31" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>29</v>
@@ -2557,10 +2508,10 @@
         <v>26</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H32" s="3">
         <v>46</v>
@@ -2569,18 +2520,18 @@
         <v>2630301</v>
       </c>
       <c r="J32" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>29</v>
@@ -2589,10 +2540,10 @@
         <v>26</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H33" s="3">
         <v>46</v>
@@ -2601,18 +2552,18 @@
         <v>8540124</v>
       </c>
       <c r="J33" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>29</v>
@@ -2621,10 +2572,10 @@
         <v>26</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H34" s="3">
         <v>47</v>
@@ -2633,18 +2584,18 @@
         <v>164025</v>
       </c>
       <c r="J34" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>29</v>
@@ -2653,10 +2604,10 @@
         <v>26</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H35" s="3">
         <v>47</v>
@@ -2665,18 +2616,18 @@
         <v>371739</v>
       </c>
       <c r="J35" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>29</v>
@@ -2685,10 +2636,10 @@
         <v>26</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H36" s="3">
         <v>48</v>
@@ -2697,18 +2648,18 @@
         <v>1369</v>
       </c>
       <c r="J36" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>29</v>
@@ -2717,10 +2668,10 @@
         <v>26</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H37" s="3">
         <v>48</v>
@@ -2729,30 +2680,30 @@
         <v>765</v>
       </c>
       <c r="J37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="H38">
         <v>49</v>
@@ -2766,25 +2717,25 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H39">
         <v>50</v>
@@ -2798,25 +2749,25 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H40">
         <v>50</v>
@@ -2860,10 +2811,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -2892,7 +2843,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -2918,7 +2869,7 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
         <v>81</v>
@@ -2944,10 +2895,10 @@
         <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -2970,7 +2921,7 @@
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -2996,7 +2947,7 @@
         <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>85</v>
@@ -3022,13 +2973,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -3048,13 +2999,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -3074,13 +3025,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -3103,13 +3054,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
@@ -3127,18 +3078,18 @@
         <v>204</v>
       </c>
       <c r="I10" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -3156,7 +3107,7 @@
         <v>206</v>
       </c>
       <c r="I11" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3192,10 +3143,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -3224,7 +3175,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -3253,7 +3204,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -3282,7 +3233,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
         <v>79</v>
@@ -3305,13 +3256,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -3334,13 +3285,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -3358,18 +3309,18 @@
         <v>165</v>
       </c>
       <c r="I6" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -3389,13 +3340,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -3415,13 +3366,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -3441,13 +3392,13 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
@@ -3467,13 +3418,13 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -3493,13 +3444,13 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
@@ -3519,13 +3470,13 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
@@ -3548,13 +3499,13 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
@@ -3585,8 +3536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0580E469-B994-456F-ADEB-B45A893DEF86}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B124" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3605,10 +3556,10 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -3632,24 +3583,24 @@
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -3664,24 +3615,24 @@
         <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>26</v>
@@ -3698,16 +3649,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -3722,7 +3673,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3730,13 +3681,13 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>26</v>
@@ -3759,16 +3710,16 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
@@ -3788,13 +3739,13 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>26</v>
@@ -3817,13 +3768,13 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>26</v>
@@ -3846,13 +3797,13 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>26</v>
@@ -3875,13 +3826,13 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>26</v>
@@ -3901,16 +3852,16 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>26</v>
@@ -3930,16 +3881,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>26</v>
@@ -3962,13 +3913,13 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>26</v>
@@ -3991,13 +3942,13 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
@@ -4020,16 +3971,16 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
@@ -4046,19 +3997,19 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>110</v>
+        <v>261</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>262</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
@@ -4075,19 +4026,19 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>263</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -4107,13 +4058,13 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>26</v>
@@ -4136,13 +4087,13 @@
         <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>26</v>
@@ -4165,13 +4116,13 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>26</v>
@@ -4191,19 +4142,19 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>26</v>
@@ -4223,13 +4174,13 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
@@ -4252,13 +4203,13 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -4281,13 +4232,13 @@
         <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
@@ -4307,13 +4258,13 @@
         <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
@@ -4333,16 +4284,16 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
@@ -4362,16 +4313,16 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="4" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E27" t="s">
         <v>26</v>
@@ -4391,16 +4342,16 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="4" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
@@ -4420,16 +4371,16 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
@@ -4452,13 +4403,13 @@
         <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
@@ -4481,13 +4432,13 @@
         <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E31" t="s">
         <v>26</v>
@@ -4507,16 +4458,16 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="4" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E32" t="s">
         <v>26</v>
@@ -4536,16 +4487,16 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E33" t="s">
         <v>26</v>
@@ -4565,16 +4516,16 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="4" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
@@ -4594,16 +4545,16 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="4" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E35" t="s">
         <v>26</v>
@@ -4623,16 +4574,16 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="4" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E36" t="s">
         <v>26</v>
@@ -4652,16 +4603,16 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="4" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E37" t="s">
         <v>26</v>
@@ -4681,16 +4632,16 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
         <v>26</v>
@@ -4713,105 +4664,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935B5A83-C9C8-4144-A52C-930CD2DF70EA}">
-  <dimension ref="B2:F22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="F3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="F4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="F5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="F6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="F7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="F8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="F9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="F10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="F11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="F12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="F13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="F14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="F15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="F16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6">
-      <c r="F17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6">
-      <c r="F22" t="str">
-        <f>F3&amp;","&amp;F4&amp;","&amp;F5&amp;","&amp;F6&amp;","&amp;F7&amp;","&amp;F8&amp;","&amp;F9&amp;","&amp;F10&amp;","&amp;F11&amp;","&amp;F12&amp;","&amp;F13&amp;","&amp;F14&amp;","&amp;F15&amp;","&amp;F16&amp;","&amp;F17</f>
-        <v>NMC333-G (Power),NMC333-G (Energy),NMC532-G (Power),NMC532-G (Energy),NMC622-G (Power),NMC622-G (Energy),NMC811-G (Power),NMC811-G (Energy),NCA-G (Power),NCA-G (Energy),LFP-G (Power),LFP-G (Energy),LMO-G (Power),LMO-G (Energy),50%/50% NMC532/LMO - G</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
squash and include large files
</commit_message>
<xml_diff>
--- a/batt_sust_model/data/battery_design_parameters.xlsx
+++ b/batt_sust_model/data/battery_design_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b8061896_newcastle_ac_uk/Documents/Python/Projects/Batt_Sust_Model-1/batt_sust_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{B116B1BF-304C-4206-9EC5-C520D68EDBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6278BAC-3BB5-4F32-8961-57F01BB450F6}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{B116B1BF-304C-4206-9EC5-C520D68EDBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C53E2F1-37C1-4B27-8CAC-525C1B306FD2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{0E16CDF7-5CB0-4173-9C6D-D5B194B1AB4C}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">cell_parameters!$A$1:$J$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">vehicle_parameters!$A$1:$J$41</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -435,9 +435,6 @@
     <t>Contains all battery design parameter names and value ranges that can be changed.</t>
   </si>
   <si>
-    <t>10,11,12,13,14,15,16,17,18</t>
-  </si>
-  <si>
     <t>6,7,8,9,10,11,12,13,14</t>
   </si>
   <si>
@@ -891,9 +888,6 @@
     <t>sep_film_thickness</t>
   </si>
   <si>
-    <t>5,6,7,8,9,10,11,12,13,14,15</t>
-  </si>
-  <si>
     <t>0,1,2,3</t>
   </si>
   <si>
@@ -1022,7 +1016,13 @@
     <t>Thickness of polymer pads between modules (default = 2), mm</t>
   </si>
   <si>
-    <t>NMC333-G (Power),NMC333-G (Energy),NMC532-G (Power),NMC532-G (Energy),NMC622-G (Power),NMC622-G (Energy),NMC811-G (Power),NMC811-G (Energy),NCA-G (Power),NCA-G (Energy),LFP-G (Power),LFP-G (Energy),LMO-G (Power),LMO-G (Energy),LMO-G (Power),50%/50% NMC532/LMO - G</t>
+    <t>NMC333-G (Power),NMC333-G (Energy),NMC532-G (Power),NMC532-G (Energy),NMC622-G (Power),NMC622-G (Energy),NMC811-G (Power),NMC811-G (Energy),NCA-G (Energy),NCA-G (Power),LFP-G (Energy),LMO-G (Energy),LMO-G (Power),50%/50% NMC532/LMO - G</t>
+  </si>
+  <si>
+    <t>10,11,12,13,14,15,16,17,18,19,20</t>
+  </si>
+  <si>
+    <t>5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="2" spans="1:1" ht="23.25">
       <c r="A2" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -1664,7 +1664,7 @@
         <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -1745,10 +1745,10 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" t="s">
         <v>254</v>
-      </c>
-      <c r="G4" t="s">
-        <v>255</v>
       </c>
       <c r="H4">
         <v>34</v>
@@ -1817,13 +1817,13 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
         <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
@@ -1843,13 +1843,13 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B8" t="s">
         <v>123</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -1867,18 +1867,18 @@
         <v>241</v>
       </c>
       <c r="J8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B9" t="s">
         <v>123</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -1896,7 +1896,7 @@
         <v>240</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1960,13 +1960,13 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
         <v>123</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>108</v>
@@ -1975,28 +1975,28 @@
         <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H12" s="3">
         <v>2</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>123</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>108</v>
@@ -2005,28 +2005,28 @@
         <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H13" s="3">
         <v>3</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18.75" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
         <v>123</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>108</v>
@@ -2035,27 +2035,27 @@
         <v>26</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14">
         <v>4</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="18.75" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B15" t="s">
         <v>123</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>29</v>
@@ -2064,27 +2064,27 @@
         <v>26</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H15">
         <v>5</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
         <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>29</v>
@@ -2093,27 +2093,27 @@
         <v>26</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H16">
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
         <v>123</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>108</v>
@@ -2122,10 +2122,10 @@
         <v>26</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H17">
         <v>14</v>
@@ -2139,13 +2139,13 @@
     </row>
     <row r="18" spans="1:10" s="3" customFormat="1">
       <c r="A18" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>108</v>
@@ -2154,10 +2154,10 @@
         <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H18" s="3">
         <v>15</v>
@@ -2171,13 +2171,13 @@
     </row>
     <row r="19" spans="1:10" s="3" customFormat="1">
       <c r="A19" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>108</v>
@@ -2186,10 +2186,10 @@
         <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H19" s="3">
         <v>16</v>
@@ -2203,13 +2203,13 @@
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1">
       <c r="A20" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>108</v>
@@ -2218,10 +2218,10 @@
         <v>26</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H20" s="3">
         <v>30</v>
@@ -2235,13 +2235,13 @@
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1">
       <c r="A21" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>108</v>
@@ -2250,10 +2250,10 @@
         <v>26</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H21" s="3">
         <v>31</v>
@@ -2267,13 +2267,13 @@
     </row>
     <row r="22" spans="1:10" s="3" customFormat="1">
       <c r="A22" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>108</v>
@@ -2282,10 +2282,10 @@
         <v>26</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H22" s="3">
         <v>32</v>
@@ -2299,13 +2299,13 @@
     </row>
     <row r="23" spans="1:10" s="3" customFormat="1">
       <c r="A23" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>108</v>
@@ -2314,10 +2314,10 @@
         <v>26</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H23" s="3">
         <v>33</v>
@@ -2331,13 +2331,13 @@
     </row>
     <row r="24" spans="1:10" s="3" customFormat="1">
       <c r="A24" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>108</v>
@@ -2346,10 +2346,10 @@
         <v>26</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H24" s="3">
         <v>34</v>
@@ -2363,13 +2363,13 @@
     </row>
     <row r="25" spans="1:10" s="3" customFormat="1">
       <c r="A25" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>108</v>
@@ -2378,10 +2378,10 @@
         <v>26</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H25" s="3">
         <v>25</v>
@@ -2395,13 +2395,13 @@
     </row>
     <row r="26" spans="1:10" s="3" customFormat="1">
       <c r="A26" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>29</v>
@@ -2410,10 +2410,10 @@
         <v>26</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H26" s="3">
         <v>36</v>
@@ -2422,18 +2422,18 @@
         <v>750</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="3" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>108</v>
@@ -2442,10 +2442,10 @@
         <v>26</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H27" s="3">
         <v>38</v>
@@ -2459,13 +2459,13 @@
     </row>
     <row r="28" spans="1:10" s="3" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>108</v>
@@ -2474,10 +2474,10 @@
         <v>26</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H28" s="3">
         <v>39</v>
@@ -2491,13 +2491,13 @@
     </row>
     <row r="29" spans="1:10" s="3" customFormat="1">
       <c r="A29" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>29</v>
@@ -2506,10 +2506,10 @@
         <v>26</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H29" s="3">
         <v>44</v>
@@ -2518,18 +2518,18 @@
         <v>2098</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
         <v>123</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>29</v>
@@ -2538,10 +2538,10 @@
         <v>26</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H30" s="3">
         <v>44</v>
@@ -2550,18 +2550,18 @@
         <v>1165</v>
       </c>
       <c r="J30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
         <v>123</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>29</v>
@@ -2570,10 +2570,10 @@
         <v>26</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H31" s="3">
         <v>45</v>
@@ -2582,18 +2582,18 @@
         <v>11990</v>
       </c>
       <c r="J31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" t="s">
         <v>123</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>29</v>
@@ -2602,10 +2602,10 @@
         <v>26</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H32" s="3">
         <v>45</v>
@@ -2614,18 +2614,18 @@
         <v>16507</v>
       </c>
       <c r="J32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
         <v>123</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>29</v>
@@ -2634,10 +2634,10 @@
         <v>26</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H33" s="3">
         <v>46</v>
@@ -2646,18 +2646,18 @@
         <v>2630301</v>
       </c>
       <c r="J33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
         <v>123</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>29</v>
@@ -2666,10 +2666,10 @@
         <v>26</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H34" s="3">
         <v>46</v>
@@ -2678,18 +2678,18 @@
         <v>8540124</v>
       </c>
       <c r="J34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
         <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>29</v>
@@ -2698,10 +2698,10 @@
         <v>26</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H35" s="3">
         <v>47</v>
@@ -2710,18 +2710,18 @@
         <v>164025</v>
       </c>
       <c r="J35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
         <v>123</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>29</v>
@@ -2730,10 +2730,10 @@
         <v>26</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H36" s="3">
         <v>47</v>
@@ -2742,18 +2742,18 @@
         <v>371739</v>
       </c>
       <c r="J36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B37" t="s">
         <v>123</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>29</v>
@@ -2762,10 +2762,10 @@
         <v>26</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H37" s="3">
         <v>48</v>
@@ -2774,18 +2774,18 @@
         <v>1369</v>
       </c>
       <c r="J37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s">
         <v>123</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>29</v>
@@ -2794,10 +2794,10 @@
         <v>26</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H38" s="3">
         <v>48</v>
@@ -2806,18 +2806,18 @@
         <v>765</v>
       </c>
       <c r="J38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B39" t="s">
         <v>123</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>108</v>
@@ -2826,10 +2826,10 @@
         <v>26</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H39">
         <v>49</v>
@@ -2843,13 +2843,13 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B40" t="s">
         <v>123</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>108</v>
@@ -2858,10 +2858,10 @@
         <v>26</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H40">
         <v>50</v>
@@ -2875,13 +2875,13 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" t="s">
         <v>123</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>108</v>
@@ -2890,10 +2890,10 @@
         <v>26</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H41">
         <v>50</v>
@@ -3100,13 +3100,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B7" t="s">
         <v>124</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -3129,13 +3129,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
         <v>124</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -3158,13 +3158,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B9" t="s">
         <v>124</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -3182,18 +3182,18 @@
         <v>205</v>
       </c>
       <c r="I9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B10" t="s">
         <v>124</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
@@ -3211,7 +3211,7 @@
         <v>207</v>
       </c>
       <c r="I10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3285,7 +3285,7 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -3305,16 +3305,16 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3334,16 +3334,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -3363,16 +3363,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -3401,7 +3401,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -3430,7 +3430,7 @@
         <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>
@@ -3447,16 +3447,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
@@ -3476,16 +3476,16 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -3500,21 +3500,21 @@
         <v>165</v>
       </c>
       <c r="I9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
         <v>26</v>
@@ -3531,16 +3531,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
@@ -3557,16 +3557,16 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -3583,16 +3583,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
@@ -3609,16 +3609,16 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
@@ -3635,16 +3635,16 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -3661,16 +3661,16 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
@@ -3690,16 +3690,16 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" t="s">
         <v>26</v>
@@ -3719,16 +3719,16 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E18" t="s">
         <v>26</v>
@@ -3745,16 +3745,16 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
         <v>26</v>
@@ -3771,16 +3771,16 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" t="s">
         <v>26</v>
@@ -3797,16 +3797,16 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C21" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E21" t="s">
         <v>26</v>
@@ -3823,16 +3823,16 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
@@ -3849,16 +3849,16 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -3875,16 +3875,16 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
@@ -3901,16 +3901,16 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C25" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
@@ -3936,7 +3936,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3999,7 +3999,7 @@
         <v>28</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
@@ -4028,10 +4028,10 @@
         <v>113</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>26</v>
@@ -4048,16 +4048,16 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>26</v>
@@ -4072,7 +4072,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -4086,7 +4086,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>26</v>
@@ -4115,10 +4115,10 @@
         <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
+        <v>291</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
@@ -4144,7 +4144,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>26</v>
@@ -4173,7 +4173,7 @@
         <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>26</v>
@@ -4202,7 +4202,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>26</v>
@@ -4231,7 +4231,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>26</v>
@@ -4260,7 +4260,7 @@
         <v>119</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>26</v>
@@ -4280,16 +4280,16 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
         <v>126</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>26</v>
@@ -4318,7 +4318,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>26</v>
@@ -4347,7 +4347,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>26</v>
@@ -4376,10 +4376,10 @@
         <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B16" t="s">
         <v>126</v>
@@ -4405,10 +4405,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>292</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
@@ -4434,10 +4434,10 @@
         <v>105</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -4454,16 +4454,16 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B18" t="s">
         <v>126</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>26</v>
@@ -4483,16 +4483,16 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B19" t="s">
         <v>126</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>26</v>
@@ -4521,7 +4521,7 @@
         <v>48</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>26</v>
@@ -4550,7 +4550,7 @@
         <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>26</v>
@@ -4579,7 +4579,7 @@
         <v>54</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>26</v>
@@ -4637,7 +4637,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" t="s">
         <v>26</v>
@@ -4666,7 +4666,7 @@
         <v>52</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
@@ -4695,7 +4695,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
@@ -4721,7 +4721,7 @@
         <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" t="s">
         <v>26</v>
@@ -4750,7 +4750,7 @@
         <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
@@ -4770,16 +4770,16 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
         <v>126</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
@@ -4799,16 +4799,16 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s">
         <v>126</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
@@ -4828,16 +4828,16 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B31" t="s">
         <v>126</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E31" t="s">
         <v>26</v>
@@ -4863,10 +4863,10 @@
         <v>126</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E32" t="s">
         <v>26</v>
@@ -4895,7 +4895,7 @@
         <v>65</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" t="s">
         <v>26</v>
@@ -4915,16 +4915,16 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B34" t="s">
         <v>126</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
@@ -4944,16 +4944,16 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
         <v>126</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E35" t="s">
         <v>26</v>
@@ -4973,16 +4973,16 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B36" t="s">
         <v>126</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E36" t="s">
         <v>26</v>
@@ -5002,16 +5002,16 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s">
         <v>126</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E37" t="s">
         <v>26</v>
@@ -5031,16 +5031,16 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B38" t="s">
         <v>126</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E38" t="s">
         <v>26</v>
@@ -5060,16 +5060,16 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s">
         <v>126</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E39" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Update the battery cost and notebook
</commit_message>
<xml_diff>
--- a/batt_sust_model/data/battery_design_parameters.xlsx
+++ b/batt_sust_model/data/battery_design_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b8061896_newcastle_ac_uk/Documents/Python/Projects/Batt_Sust_Model-1/batt_sust_model/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joris\OneDrive - Newcastle University\Python\Projects\Batt_Sust_Model-1\batt_sust_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{B116B1BF-304C-4206-9EC5-C520D68EDBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C53E2F1-37C1-4B27-8CAC-525C1B306FD2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39AE1E-7100-4102-872D-E380505DE821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{0E16CDF7-5CB0-4173-9C6D-D5B194B1AB4C}"/>
   </bookViews>
@@ -1022,7 +1022,7 @@
     <t>10,11,12,13,14,15,16,17,18,19,20</t>
   </si>
   <si>
-    <t>5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20</t>
+    <t>5,7,9,11,13,15,17,19</t>
   </si>
 </sst>
 </file>
@@ -3936,7 +3936,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>